<commit_message>
UiPath Demo -Dispatcher Bot
UiPath Demo -Dispatcher Bot

Adds the data from the excel sheet to the Queue present in the Orchestrator
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\UiPath\UiPathDemo_GITIntegration\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\GitHub\UiPathDemo-UiPath_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB161891-1070-4D80-A119-19155558FAE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2823C372-9CD5-4D20-ADFE-B374F307462B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="48" windowWidth="17304" windowHeight="12312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="48" windowWidth="17304" windowHeight="12312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -98,10 +98,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
   </si>
   <si>
@@ -123,17 +119,20 @@
     <t>InputFile</t>
   </si>
   <si>
-    <t>C:\Users\HP\Documents\UiPath\UiPathDemo_GITIntegration\Data\Input\Transactions.xlsx</t>
+    <t>UiDemoQueue</t>
   </si>
   <si>
-    <t>UiDemoQueue</t>
+    <t>C:\Users\HP\Documents\Input Files - UiDemo\Transactions.xlsx</t>
+  </si>
+  <si>
+    <t>OrchestratorQueueName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -157,6 +156,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -178,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -188,6 +193,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,7 +511,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -552,10 +558,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B2" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -576,7 +582,7 @@
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B6" t="s">
         <v>32</v>
@@ -1636,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1660,7 +1666,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
@@ -1682,7 +1688,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
@@ -1693,7 +1699,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
@@ -1704,7 +1710,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2714,7 +2720,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Updated the Inputfile Location
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\UiPath\UiPathDemo_GITIntegration\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\UiPath\Codes\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB161891-1070-4D80-A119-19155558FAE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6908CC62-7875-4F7D-8C8D-013155E188A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="48" windowWidth="17304" windowHeight="12312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>Name</t>
   </si>
@@ -123,10 +123,16 @@
     <t>InputFile</t>
   </si>
   <si>
-    <t>C:\Users\HP\Documents\UiPath\UiPathDemo_GITIntegration\Data\Input\Transactions.xlsx</t>
+    <t>OrchestratorFolderName</t>
   </si>
   <si>
-    <t>UiDemoQueue</t>
+    <t>MyTestQueue</t>
+  </si>
+  <si>
+    <t>My_Folder</t>
+  </si>
+  <si>
+    <t>C:\Users\HP\Documents\UiPath\Codes\Data\Input\Transactions.xlsx</t>
   </si>
 </sst>
 </file>
@@ -179,10 +185,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -505,7 +511,7 @@
   <dimension ref="A1:Z997"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -561,7 +567,14 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="3" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+    </row>
     <row r="4" spans="1:26" ht="28.8">
       <c r="A4" t="s">
         <v>20</v>
@@ -579,7 +592,7 @@
         <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>